<commit_message>
Adjust standard deviation calculation
</commit_message>
<xml_diff>
--- a/Homework/HW5/simulation result(prob4-b).xlsx
+++ b/Homework/HW5/simulation result(prob4-b).xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanbaep2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanbaep2/Desktop/FIN513/Homework/HW5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="4480" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="8200" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,6 +361,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -385,13 +386,14 @@
         <v>0.2</v>
       </c>
       <c r="B2" s="2">
-        <v>1.7631899999999999E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>7.7898400000000003E-4</v>
+        <v>1.7259199999999999E-2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.17688799999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>22.634599999999999</v>
+        <f>B2 / C2</f>
+        <v>9.7571344579621008E-2</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -400,13 +402,15 @@
         <v>0.3</v>
       </c>
       <c r="B3" s="2">
-        <v>2.2982200000000001E-2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.8646800000000001E-3</v>
+        <v>2.62832E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f>0.430704</f>
+        <v>0.43070399999999998</v>
       </c>
       <c r="D3" s="1">
-        <v>12.324999999999999</v>
+        <f>B3 / C3</f>
+        <v>6.1023812177272561E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -414,13 +418,14 @@
         <v>0.4</v>
       </c>
       <c r="B4" s="2">
-        <v>3.2071000000000002E-2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3.7791700000000001E-3</v>
+        <v>3.1419000000000002E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.89496699999999996</v>
       </c>
       <c r="D4" s="1">
-        <v>8.4862300000000008</v>
+        <f>B4 / C4</f>
+        <v>3.5106322356019834E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -428,13 +433,14 @@
         <v>0.5</v>
       </c>
       <c r="B5" s="2">
-        <v>6.05563E-2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9.0087299999999995E-3</v>
+        <v>6.0172799999999999E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.7873000000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>6.7219600000000002</v>
+        <f>B5 / C5</f>
+        <v>3.3666871817825766E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>